<commit_message>
Damage and Selfdestructed Logic - without test
</commit_message>
<xml_diff>
--- a/unitdata.xlsx
+++ b/unitdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liu.zehu\Documents\SIFIWARCHESS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFFA614-406F-4313-8F59-0AF184660B4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C907CDAD-C739-4B5E-B842-AE6EE4F0B8F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="48">
   <si>
     <t>name</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>g_hm</t>
+  </si>
+  <si>
+    <t>a_hm</t>
   </si>
 </sst>
 </file>
@@ -634,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:X33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -827,7 +830,7 @@
         <v>41</v>
       </c>
       <c r="V6" s="14" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="W6" s="15" t="s">
         <v>25</v>
@@ -1140,7 +1143,7 @@
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B31" s="14" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C31" s="20">
         <v>6</v>

</xml_diff>